<commit_message>
Finish Customer Detail, working on added Invoice from cart
</commit_message>
<xml_diff>
--- a/Data Dictionary.xlsx
+++ b/Data Dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\C# 2\Final Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cardo\Desktop\repos\MusicStore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BDB06DF-BF0C-47A3-A1D0-3EC8535D76B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E26B618-F3BD-45FC-BDE4-179337DB5D85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4170" yWindow="1260" windowWidth="21600" windowHeight="11385" tabRatio="981" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="5190" yWindow="5835" windowWidth="18210" windowHeight="8340" tabRatio="981" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="137">
   <si>
     <t>FIELD</t>
   </si>
@@ -439,9 +439,6 @@
   </si>
   <si>
     <t>InvoiceID</t>
-  </si>
-  <si>
-    <t>InvoiceLine.InvoiceLineID</t>
   </si>
   <si>
     <t>Date</t>
@@ -888,11 +885,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O115"/>
+  <dimension ref="A1:O114"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B119" sqref="B119"/>
+      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A113" sqref="A113:XFD113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3115,15 +3112,15 @@
       </c>
       <c r="O112" s="13"/>
     </row>
-    <row r="113" spans="1:15" s="12" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A113" s="10" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B113" s="11" t="s">
-        <v>10</v>
+        <v>97</v>
       </c>
       <c r="D113" s="12" t="s">
-        <v>28</v>
+        <v>116</v>
       </c>
       <c r="H113" s="12" t="s">
         <v>28</v>
@@ -3134,24 +3131,22 @@
       <c r="J113" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="L113" s="11" t="s">
-        <v>26</v>
-      </c>
+      <c r="L113" s="11"/>
       <c r="M113" s="11"/>
-      <c r="N113" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="O113" s="13"/>
+      <c r="N113" s="11"/>
+      <c r="O113" s="13" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="114" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A114" s="10" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B114" s="11" t="s">
-        <v>97</v>
+        <v>51</v>
       </c>
       <c r="D114" s="12" t="s">
-        <v>116</v>
+        <v>28</v>
       </c>
       <c r="H114" s="12" t="s">
         <v>28</v>
@@ -3166,33 +3161,7 @@
       <c r="M114" s="11"/>
       <c r="N114" s="11"/>
       <c r="O114" s="13" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="115" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="10" t="s">
         <v>136</v>
-      </c>
-      <c r="B115" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D115" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="H115" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I115" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="J115" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L115" s="11"/>
-      <c r="M115" s="11"/>
-      <c r="N115" s="11"/>
-      <c r="O115" s="13" t="s">
-        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>